<commit_message>
Update to match v2.3 folder structure
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
+++ b/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa-SET_master\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa-SET-MTS\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3070AB0C-8CC5-4642-BBBE-7FCC24106826}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A64348D-7939-47FA-B86D-82B305B336D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1001,7 +1001,7 @@
   <dimension ref="A1:H165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1165,7 +1165,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>135</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>39</v>
       </c>
       <c r="C32" s="18">
-        <v>42735</v>
+        <v>42384</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
Small fix for gdx_handler where no GAMS path is provided
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
+++ b/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa-SET-MTS\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A64348D-7939-47FA-B86D-82B305B336D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5270CDD-3370-451A-9BBF-2F72116A4288}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1000,8 +1000,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1757,7 +1757,7 @@
         <v>6</v>
       </c>
       <c r="C93" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
New build_dispaset_simulation wrapper function. Different  Mid-term-scheduling options callable from Config file. None, Standard and Standard + desired zones
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
+++ b/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa-SET-MTS\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5270CDD-3370-451A-9BBF-2F72116A4288}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E22FBE-D886-4EC7-8072-90FAE6992FE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
     <sheet name="ReserveParticipation" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$48:$C$50</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="160">
   <si>
     <t>Default value</t>
   </si>
@@ -490,6 +493,18 @@
   </si>
   <si>
     <t>Simulations/simulation_MidTermScheduling</t>
+  </si>
+  <si>
+    <t>Hydro scheduling</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>These parameters influence how HDAM and HPHS units are operated (e.g. if Standard: scaled reservoir levels are computed internally</t>
+  </si>
+  <si>
+    <t>Rolling</t>
   </si>
 </sst>
 </file>
@@ -528,7 +543,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -544,6 +559,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -649,6 +670,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1000,8 +1030,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1018,16 +1048,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -1041,15 +1071,15 @@
     </row>
     <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
@@ -1065,15 +1095,15 @@
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
@@ -1209,7 +1239,7 @@
         <v>39</v>
       </c>
       <c r="C32" s="18">
-        <v>42384</v>
+        <v>42400</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>75</v>
@@ -1298,7 +1328,20 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:8" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B50" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="H50" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
     <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1394,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="5">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="H66" s="11" t="s">
         <v>73</v>
@@ -1672,7 +1715,7 @@
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A88" s="26" t="s">
+      <c r="A88" s="29" t="s">
         <v>53</v>
       </c>
       <c r="B88" s="6" t="s">
@@ -1692,7 +1735,7 @@
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A89" s="26"/>
+      <c r="A89" s="29"/>
       <c r="B89" s="6" t="s">
         <v>138</v>
       </c>
@@ -1707,7 +1750,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A90" s="26"/>
+      <c r="A90" s="29"/>
       <c r="B90" s="6" t="s">
         <v>5</v>
       </c>
@@ -1722,12 +1765,12 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A91" s="26"/>
+      <c r="A91" s="29"/>
       <c r="B91" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C91" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>19</v>
@@ -1737,7 +1780,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A92" s="26"/>
+      <c r="A92" s="29"/>
       <c r="B92" s="6" t="s">
         <v>16</v>
       </c>
@@ -1752,12 +1795,12 @@
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A93" s="26"/>
+      <c r="A93" s="29"/>
       <c r="B93" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C93" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>21</v>
@@ -1767,12 +1810,12 @@
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="26"/>
+      <c r="A94" s="29"/>
       <c r="B94" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C94" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>139</v>
@@ -1782,7 +1825,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A95" s="26"/>
+      <c r="A95" s="29"/>
       <c r="B95" s="6" t="s">
         <v>7</v>
       </c>
@@ -1797,7 +1840,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A96" s="26"/>
+      <c r="A96" s="29"/>
       <c r="B96" s="6" t="s">
         <v>9</v>
       </c>
@@ -1812,7 +1855,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A97" s="26"/>
+      <c r="A97" s="29"/>
       <c r="B97" s="6" t="s">
         <v>11</v>
       </c>
@@ -1827,7 +1870,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A98" s="26"/>
+      <c r="A98" s="29"/>
       <c r="B98" s="6" t="s">
         <v>12</v>
       </c>
@@ -1842,7 +1885,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A99" s="26"/>
+      <c r="A99" s="29"/>
       <c r="B99" s="6" t="s">
         <v>28</v>
       </c>
@@ -1857,12 +1900,12 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A100" s="26"/>
+      <c r="A100" s="29"/>
       <c r="B100" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C100" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>26</v>
@@ -1872,7 +1915,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A101" s="26"/>
+      <c r="A101" s="29"/>
       <c r="B101" s="6" t="s">
         <v>14</v>
       </c>
@@ -1887,7 +1930,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="26"/>
+      <c r="A102" s="29"/>
       <c r="B102" s="6" t="s">
         <v>20</v>
       </c>
@@ -2155,7 +2198,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000011000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
@@ -2198,6 +2241,12 @@
           </x14:formula1>
           <xm:sqref>C47</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{86FAD3D9-F1C3-47D5-A81B-4788D9BD562F}">
+          <x14:formula1>
+            <xm:f>Lists!$E$2:$E$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>C50</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2207,10 +2256,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2219,9 +2268,10 @@
     <col min="2" max="2" width="32.5546875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>4</v>
       </c>
@@ -2234,8 +2284,11 @@
       <c r="D1" s="17" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2248,8 +2301,11 @@
       <c r="D2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2259,16 +2315,22 @@
       <c r="D3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>46</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>137</v>
       </c>
@@ -2276,7 +2338,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>140</v>
       </c>

</xml_diff>

<commit_message>
Cleanup and minor fixes for paths and functions
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
+++ b/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa-SET-MTS\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E22FBE-D886-4EC7-8072-90FAE6992FE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA3C875-2998-4BD2-B066-E207516BD45C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="159">
   <si>
     <t>Default value</t>
   </si>
@@ -498,13 +498,10 @@
     <t>Hydro scheduling</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>These parameters influence how HDAM and HPHS units are operated (e.g. if Standard: scaled reservoir levels are computed internally</t>
   </si>
   <si>
-    <t>Rolling</t>
+    <t>Off</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1027,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
@@ -1339,7 +1336,7 @@
         <v>141</v>
       </c>
       <c r="H50" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2258,8 +2255,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2302,7 +2299,7 @@
         <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2325,9 +2322,6 @@
       </c>
       <c r="D4" t="s">
         <v>84</v>
-      </c>
-      <c r="E4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added option for regional hydro scheduling, now there are 3 options: Off - standard, Zonal - computed for each zone individually, Regional - computed for whole region at once
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
+++ b/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa-SET-MTS\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA3C875-2998-4BD2-B066-E207516BD45C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE885BE-B767-418A-8AB4-63F27821A66D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="161">
   <si>
     <t>Default value</t>
   </si>
@@ -502,6 +502,12 @@
   </si>
   <si>
     <t>Off</t>
+  </si>
+  <si>
+    <t>Regional</t>
+  </si>
+  <si>
+    <t>Zonal</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1033,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
@@ -1333,7 +1339,7 @@
         <v>62</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="H50" s="26" t="s">
         <v>157</v>
@@ -2255,7 +2261,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -2313,7 +2319,7 @@
         <v>87</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2322,6 +2328,9 @@
       </c>
       <c r="D4" t="s">
         <v>84</v>
+      </c>
+      <c r="E4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Improved descriptions and new selection options added to the Config file.
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
+++ b/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
@@ -8,24 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa-SET-MTS\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE885BE-B767-418A-8AB4-63F27821A66D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81521695-CBA5-4813-821C-A8BD51D77416}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
     <sheet name="ReserveParticipation" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$48:$C$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$48:$C$54</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="197">
   <si>
     <t>Default value</t>
   </si>
@@ -453,15 +456,9 @@
     <t>Standard</t>
   </si>
   <si>
-    <t>Price of unserved heat</t>
-  </si>
-  <si>
     <t>Load Shedding Cost</t>
   </si>
   <si>
-    <t xml:space="preserve">NB: Ireland (IE) includes north Ireland. </t>
-  </si>
-  <si>
     <t>NB: UK is not considered as zone but GB is.</t>
   </si>
   <si>
@@ -508,13 +505,127 @@
   </si>
   <si>
     <t>Zonal</t>
+  </si>
+  <si>
+    <t>Price of Spillage</t>
+  </si>
+  <si>
+    <t>Price of Unserved Heat</t>
+  </si>
+  <si>
+    <t>Value of Lost Load (VOLL)</t>
+  </si>
+  <si>
+    <t>Water Value</t>
+  </si>
+  <si>
+    <t>Cost occurring due to involuntary water spillage in hydro resrvoirs EUR/MWh</t>
+  </si>
+  <si>
+    <t>Value of water (for unsatisfied water reservoir levels) EUR/MWh</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>LI</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>MK</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>UA</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>XK</t>
+  </si>
+  <si>
+    <t>Hydro scheduling horizon</t>
+  </si>
+  <si>
+    <t>Stop-date driven</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>These parameters influence the horizon of the hydro scheduling (e.g. if Annual: reservoirs are computed for the whole year, if Stop-date driven: computation of reservoirs is driven by the start and stop date</t>
+  </si>
+  <si>
+    <t>Simulation Options</t>
+  </si>
+  <si>
+    <t>Input Data</t>
+  </si>
+  <si>
+    <t>Horizon Settings</t>
+  </si>
+  <si>
+    <t>Scenario Options</t>
+  </si>
+  <si>
+    <t>Zone Options</t>
+  </si>
+  <si>
+    <t>Reserve Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NB: Ireland (IE) includes Northern Ireland. </t>
+  </si>
+  <si>
+    <t>Hydro Scheduling Options</t>
+  </si>
+  <si>
+    <t>Between 0 - 1</t>
+  </si>
+  <si>
+    <t>-&gt; Initial level</t>
+  </si>
+  <si>
+    <t>&lt;- Final level</t>
+  </si>
+  <si>
+    <t>Initial/Final resevoir levels</t>
+  </si>
+  <si>
+    <t>The highest amount that customers would be willing to pay to avoid a disruption in their electricity service. EUR/MWh</t>
+  </si>
+  <si>
+    <t>The least amount that customers are willing to recieve to reduce the electricity demand. EUR/MWh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,8 +656,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -567,12 +693,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFACC0AC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9D7A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -598,11 +742,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -674,23 +829,74 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -698,6 +904,15 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE9D7A6"/>
+      <color rgb="FFA1A295"/>
+      <color rgb="FFACC0AC"/>
+      <color rgb="FFECBE8B"/>
+      <color rgb="FFD9AE8F"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -707,6 +922,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Lists"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1033,13 +1261,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.109375" style="1" customWidth="1"/>
@@ -1051,18 +1279,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-    </row>
-    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+    </row>
+    <row r="2" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1072,17 +1300,18 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="29" t="s">
+    <row r="3" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:8" s="46" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="44"/>
+      <c r="B4" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
@@ -1095,20 +1324,20 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-    </row>
-    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1117,7 +1346,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="8" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="C8" s="14"/>
     </row>
@@ -1129,16 +1358,27 @@
     <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+    </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D18" s="13"/>
       <c r="H18" s="1" t="s">
@@ -1149,7 +1389,7 @@
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="34" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="4" t="b">
@@ -1163,7 +1403,7 @@
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="34" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="4" t="b">
@@ -1177,7 +1417,7 @@
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="34" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="4" t="b">
@@ -1191,7 +1431,7 @@
       <c r="A22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="33" t="s">
         <v>89</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -1202,7 +1442,7 @@
       <c r="A23" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="33" t="s">
         <v>89</v>
       </c>
       <c r="C23" s="4"/>
@@ -1215,16 +1455,24 @@
     <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="C30" s="14"/>
+      <c r="A30" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="32" t="s">
         <v>39</v>
       </c>
       <c r="C31" s="18">
@@ -1238,7 +1486,7 @@
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="32" t="s">
         <v>39</v>
       </c>
       <c r="C32" s="18">
@@ -1252,7 +1500,7 @@
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="32" t="s">
         <v>48</v>
       </c>
       <c r="C33" s="4">
@@ -1266,13 +1514,14 @@
       <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="32" t="s">
         <v>48</v>
       </c>
       <c r="C34" s="4">
         <v>1</v>
       </c>
     </row>
+    <row r="35" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1283,8 +1532,16 @@
     <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:8" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
-      <c r="C45" s="14"/>
+      <c r="A45" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
     </row>
     <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
@@ -1293,7 +1550,7 @@
       <c r="A47" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="34" t="s">
         <v>62</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -1307,7 +1564,7 @@
       <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="34" t="s">
         <v>62</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -1321,7 +1578,7 @@
       <c r="A49" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="34" t="s">
         <v>4</v>
       </c>
       <c r="C49" s="4" t="b">
@@ -1331,61 +1588,135 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="B50" s="26" t="s">
+    <row r="50" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:8" s="8" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" s="38"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+    </row>
+    <row r="54" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C50" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="H50" s="26" t="s">
+      <c r="C54" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:8" s="10" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H54" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E57" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E58" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F58" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:8" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
       <c r="C60" s="15"/>
     </row>
-    <row r="61" spans="1:8" s="8" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="7"/>
-      <c r="C61" s="14"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="B61" s="38"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="38"/>
+    </row>
+    <row r="62" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>92</v>
       </c>
       <c r="H62" s="11"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>92</v>
@@ -1394,15 +1725,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D64" s="19" t="s">
         <v>92</v>
@@ -1411,32 +1742,29 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D65" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C66" s="20"/>
+      <c r="C66" s="47"/>
       <c r="D66" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" s="32" t="s">
         <v>0</v>
       </c>
       <c r="F66" s="5">
@@ -1446,15 +1774,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D67" s="19" t="s">
         <v>92</v>
@@ -1463,15 +1791,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D68" s="19" t="s">
         <v>92</v>
@@ -1480,15 +1808,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D69" s="19" t="s">
         <v>92</v>
@@ -1497,52 +1825,52 @@
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C70" s="20"/>
       <c r="D70" s="19"/>
-      <c r="E70" s="1" t="s">
+      <c r="E70" s="32" t="s">
         <v>0</v>
       </c>
       <c r="F70" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C71" s="20"/>
       <c r="D71" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" s="32" t="s">
         <v>0</v>
       </c>
       <c r="F71" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C72" s="20"/>
       <c r="D72" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" s="32" t="s">
         <v>0</v>
       </c>
       <c r="F72" s="5">
@@ -1552,54 +1880,54 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C73" s="20"/>
       <c r="D73" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E73" s="32" t="s">
         <v>0</v>
       </c>
       <c r="F73" s="5">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C74" s="20"/>
       <c r="D74" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" s="32" t="s">
         <v>0</v>
       </c>
       <c r="F74" s="5">
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C75" s="20"/>
       <c r="D75" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" s="32" t="s">
         <v>0</v>
       </c>
       <c r="F75" s="5">
@@ -1610,57 +1938,57 @@
       <c r="A76" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D76" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C77" s="20"/>
       <c r="D77" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" s="32" t="s">
         <v>0</v>
       </c>
       <c r="F77" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C78" s="20"/>
       <c r="D78" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E78" s="32" t="s">
         <v>0</v>
       </c>
       <c r="F78" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C79" s="20"/>
@@ -1668,308 +1996,464 @@
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B80" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B80" s="33" t="s">
         <v>37</v>
       </c>
       <c r="C80" s="20"/>
       <c r="D80" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E80" s="32" t="s">
         <v>0</v>
       </c>
       <c r="F80" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C81" s="20"/>
+        <v>142</v>
+      </c>
+      <c r="C81" s="47"/>
       <c r="D81" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E81" s="32" t="s">
         <v>0</v>
       </c>
       <c r="F81" s="5">
         <v>400</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" spans="1:8" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" spans="1:8" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H81" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="E82" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F82" s="25">
+        <v>100000</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="E83" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F83" s="5">
+        <v>1</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="E84" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F84" s="5">
+        <v>100</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="9"/>
       <c r="C85" s="15"/>
     </row>
-    <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="B86" s="41"/>
+      <c r="C86" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="41"/>
+      <c r="E86" s="41"/>
+      <c r="F86" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G86" s="41"/>
+      <c r="H86" s="41"/>
+    </row>
+    <row r="87" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A88" s="29" t="s">
+      <c r="B87" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C87" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F87" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="27" t="s">
         <v>53</v>
       </c>
       <c r="B88" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C88" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F88" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="27"/>
+      <c r="B89" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C88" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="6" t="s">
+      <c r="C89" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="27"/>
+      <c r="B90" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C90" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F90" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="27"/>
+      <c r="B91" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C91" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F91" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="27"/>
+      <c r="B92" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F92" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="27"/>
+      <c r="B93" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C93" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="F93" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="27"/>
+      <c r="B94" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C94" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F94" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="27"/>
+      <c r="B95" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F95" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="27"/>
+      <c r="B96" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F96" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="27"/>
+      <c r="B97" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F97" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="27"/>
+      <c r="B98" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F98" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="27"/>
+      <c r="B99" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F99" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="27"/>
+      <c r="B100" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F100" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="27"/>
+      <c r="B101" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F101" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="27"/>
+      <c r="B102" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C102" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F102" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C103" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F103" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C104" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F104" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C105" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F105" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="B106" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F88" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A89" s="29"/>
-      <c r="B89" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C89" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="6" t="s">
+      <c r="C106" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="F106" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="31"/>
+      <c r="B107" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C107" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F107" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F89" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A90" s="29"/>
-      <c r="B90" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F90" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A91" s="29"/>
-      <c r="B91" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C91" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F91" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A92" s="29"/>
-      <c r="B92" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C92" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F92" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A93" s="29"/>
-      <c r="B93" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C93" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F93" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="29"/>
-      <c r="B94" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C94" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F94" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A95" s="29"/>
-      <c r="B95" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C95" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F95" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A96" s="29"/>
-      <c r="B96" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C96" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F96" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A97" s="29"/>
-      <c r="B97" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C97" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F97" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A98" s="29"/>
-      <c r="B98" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C98" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F98" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A99" s="29"/>
-      <c r="B99" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C99" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F99" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A100" s="29"/>
-      <c r="B100" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C100" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E100" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F100" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A101" s="29"/>
-      <c r="B101" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C101" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E101" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F101" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="29"/>
-      <c r="B102" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C102" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E102" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F102" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H102" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="105" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="108" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="9"/>
-      <c r="C109" s="15"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
+      <c r="C108" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F108" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" s="29" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="28"/>
+      <c r="C109" s="30"/>
+    </row>
+    <row r="110" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="37" t="s">
         <v>76</v>
       </c>
+      <c r="B111" s="38"/>
+      <c r="C111" s="39"/>
+      <c r="D111" s="38"/>
+      <c r="E111" s="38"/>
+      <c r="F111" s="38"/>
+      <c r="G111" s="38"/>
+      <c r="H111" s="38"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="32" t="s">
         <v>79</v>
       </c>
       <c r="C112" s="5">
@@ -1980,7 +2464,7 @@
       <c r="A113" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="32" t="s">
         <v>79</v>
       </c>
       <c r="C113" s="5">
@@ -1994,7 +2478,7 @@
       <c r="A114" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" s="32" t="s">
         <v>79</v>
       </c>
       <c r="C114" s="5">
@@ -2008,14 +2492,14 @@
       <c r="A115" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="32" t="s">
         <v>79</v>
       </c>
       <c r="C115" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
@@ -2027,16 +2511,32 @@
     <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="128" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="9"/>
       <c r="C128" s="15"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" s="2" t="s">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A130" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="B130" s="41"/>
+      <c r="C130" s="42"/>
+      <c r="D130" s="41"/>
+      <c r="E130" s="41"/>
+      <c r="F130" s="41"/>
+      <c r="G130" s="41"/>
+      <c r="H130" s="41"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C131" s="35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B132" s="23" t="s">
         <v>95</v>
       </c>
@@ -2044,7 +2544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B133" s="23" t="s">
         <v>96</v>
       </c>
@@ -2052,7 +2552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B134" s="23" t="s">
         <v>97</v>
       </c>
@@ -2060,7 +2560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B135" s="23" t="s">
         <v>98</v>
       </c>
@@ -2068,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B136" s="23" t="s">
         <v>99</v>
       </c>
@@ -2076,7 +2576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B137" s="23" t="s">
         <v>100</v>
       </c>
@@ -2084,7 +2584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B138" s="23" t="s">
         <v>101</v>
       </c>
@@ -2092,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B139" s="23" t="s">
         <v>102</v>
       </c>
@@ -2100,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B140" s="23" t="s">
         <v>103</v>
       </c>
@@ -2108,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B141" s="23" t="s">
         <v>104</v>
       </c>
@@ -2116,7 +2616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B142" s="23" t="s">
         <v>105</v>
       </c>
@@ -2124,7 +2624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B143" s="23" t="s">
         <v>106</v>
       </c>
@@ -2132,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B144" s="23" t="s">
         <v>107</v>
       </c>
@@ -2160,13 +2660,15 @@
       <c r="F165" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="A88:A102"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B4:H4"/>
+    <mergeCell ref="A106:A107"/>
   </mergeCells>
-  <dataValidations count="17">
+  <phoneticPr fontId="5" type="noConversion"/>
+  <dataValidations count="21">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C18:D18" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -2177,13 +2679,13 @@
       <formula2>73051</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C68" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F70:F74 F77:F78 F80:F81" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F70:F74 F77:F78 F80" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C112" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C113" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C114" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C115" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C22" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F66" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F66 F57:F58" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F75" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C23" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C69" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
@@ -2196,17 +2698,21 @@
       <formula1>1</formula1>
       <formula2>365</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Load Shedding Costs" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F81" xr:uid="{1195FB7B-37A6-4912-A3EE-96C2F97F346B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Value of Lost Load" prompt="Value of Lost Load represents the highest ammount that customers would be willing to pay to avoid disruption. Should be set to a really high value (e.a. &gt;10e5) " sqref="F82" xr:uid="{A011503E-FACE-460E-BFDF-1701CC622931}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Price of spillage" prompt="Involuntary water spillage in hydro reservirs. Relativley low value (e.a. &lt;5)" sqref="F83" xr:uid="{55DE26F7-FB99-4503-A869-CFB48A9FAFFA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Water Value" prompt="Value of water for unsatisfied reservoir levels. High number (e.a. 100 &lt; x &lt; 400)" sqref="F84" xr:uid="{93C10F4D-B06D-4B18-B580-B5E72EA43594}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000011000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F88:G102 C88:C102 C132:C146</xm:sqref>
+          <xm:sqref>C132:C146 C87:C108 F87:F108</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write excel files" prompt="If set to true, one excel file per parameter will be written in the simulation environment directory." xr:uid="{00000000-0002-0000-0000-000012000000}">
           <x14:formula1>
@@ -2244,11 +2750,29 @@
           </x14:formula1>
           <xm:sqref>C47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{86FAD3D9-F1C3-47D5-A81B-4788D9BD562F}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hydro Scheduling" prompt="Select type of mid-term hydro scheduling._x000a_Off: Mid-term scheduling is not performed, hystorical reservoir levels are used instead_x000a_Regional: Performed for the whole region simultaneously_x000a_Zonal: Performed for each zone individually" xr:uid="{86FAD3D9-F1C3-47D5-A81B-4788D9BD562F}">
           <x14:formula1>
             <xm:f>Lists!$E$2:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C50</xm:sqref>
+          <xm:sqref>C54</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0512806B-C050-4E95-821E-3CF48A786E8B}">
+          <x14:formula1>
+            <xm:f>[ConfigEU.xlsx]Lists!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>G88:G102</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hydro scheduling horizon" prompt="Annual: Performes hydro scheduling for one year_x000a_Stop-date driven: Performes hydro scheduling between Start and Stop dates_x000a_" xr:uid="{345F7B42-F54C-4808-919E-6CF06ADB107C}">
+          <x14:formula1>
+            <xm:f>Lists!$F$2:$F$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C55</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Initial/Final reservoir levels" prompt="Values for the initial and final levels, usefull when no reservoir levels are proided as inputs in the Input data" xr:uid="{A38CDE04-BA26-4377-B449-1F28F030BC87}">
+          <x14:formula1>
+            <xm:f>Lists!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C56</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2259,10 +2783,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2274,7 +2798,7 @@
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>4</v>
       </c>
@@ -2288,10 +2812,13 @@
         <v>83</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2305,10 +2832,13 @@
         <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+      <c r="F2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2319,10 +2849,13 @@
         <v>87</v>
       </c>
       <c r="E3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+      <c r="F3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -2330,10 +2863,10 @@
         <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>137</v>
       </c>
@@ -2341,7 +2874,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>140</v>
       </c>
@@ -2358,7 +2891,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated GAMS files to output Water Value (dual of storage balance constraint) and lost load due to unsatisfied reservoir constraints in the last time step
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
+++ b/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa-SET-MTS\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81521695-CBA5-4813-821C-A8BD51D77416}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D130CF7-97AA-4B95-9F96-567DF3CCE4A4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="196">
   <si>
     <t>Default value</t>
   </si>
@@ -601,9 +601,6 @@
   </si>
   <si>
     <t>Hydro Scheduling Options</t>
-  </si>
-  <si>
-    <t>Between 0 - 1</t>
   </si>
   <si>
     <t>-&gt; Initial level</t>
@@ -1262,7 +1259,7 @@
   <dimension ref="A1:H165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1639,7 +1636,7 @@
     </row>
     <row r="56" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B56" s="34" t="s">
         <v>4</v>
@@ -1650,9 +1647,6 @@
     </row>
     <row r="57" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="36" t="s">
-        <v>192</v>
-      </c>
-      <c r="B57" s="1" t="s">
         <v>191</v>
       </c>
       <c r="E57" s="32" t="s">
@@ -1664,10 +1658,7 @@
     </row>
     <row r="58" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E58" s="32" t="s">
         <v>0</v>
@@ -2029,7 +2020,7 @@
         <v>400</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2044,7 +2035,7 @@
         <v>100000</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2668,7 +2659,7 @@
     <mergeCell ref="A106:A107"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <dataValidations count="21">
+  <dataValidations count="23">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C18:D18" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -2685,7 +2676,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C114" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C115" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C22" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F66 F57:F58" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F66" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F75" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C23" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C69" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
@@ -2702,6 +2693,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Value of Lost Load" prompt="Value of Lost Load represents the highest ammount that customers would be willing to pay to avoid disruption. Should be set to a really high value (e.a. &gt;10e5) " sqref="F82" xr:uid="{A011503E-FACE-460E-BFDF-1701CC622931}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Price of spillage" prompt="Involuntary water spillage in hydro reservirs. Relativley low value (e.a. &lt;5)" sqref="F83" xr:uid="{55DE26F7-FB99-4503-A869-CFB48A9FAFFA}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Water Value" prompt="Value of water for unsatisfied reservoir levels. High number (e.a. 100 &lt; x &lt; 400)" sqref="F84" xr:uid="{93C10F4D-B06D-4B18-B580-B5E72EA43594}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max storage)" prompt="Initial state of charge. It is defined as the % of total storage capacity." sqref="F57" xr:uid="{C22C312A-4C0D-465E-AA40-04829D4E1DD5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max storage)" prompt="FInal state of charge. It is defined as the % of total storage capacity." sqref="F58" xr:uid="{70E3A2FC-178F-4589-82CF-31382B011A9B}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Preprocessing now updated to include different options for initial and final reservoir levels
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
+++ b/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa-SET-MTS\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D130CF7-97AA-4B95-9F96-567DF3CCE4A4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5227D2FB-F1F6-4379-905F-DF761FABC670}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -622,7 +622,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -654,16 +654,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <u/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -754,7 +761,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -829,71 +836,86 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1258,8 +1280,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1276,16 +1298,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -1298,17 +1320,17 @@
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:8" s="46" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45" t="s">
+    <row r="4" spans="1:8" s="35" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34"/>
+      <c r="B4" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
@@ -1321,18 +1343,18 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
@@ -1355,23 +1377,23 @@
     <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37" t="s">
+    <row r="17" spans="1:8" s="45" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1386,7 +1408,7 @@
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="31" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="4" t="b">
@@ -1400,7 +1422,7 @@
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="31" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="4" t="b">
@@ -1414,7 +1436,7 @@
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="31" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="4" t="b">
@@ -1428,7 +1450,7 @@
       <c r="A22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="30" t="s">
         <v>89</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -1439,7 +1461,7 @@
       <c r="A23" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="30" t="s">
         <v>89</v>
       </c>
       <c r="C23" s="4"/>
@@ -1453,23 +1475,23 @@
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="37" t="s">
+    <row r="30" spans="1:8" s="45" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="29" t="s">
         <v>39</v>
       </c>
       <c r="C31" s="18">
@@ -1483,7 +1505,7 @@
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="29" t="s">
         <v>39</v>
       </c>
       <c r="C32" s="18">
@@ -1497,7 +1519,7 @@
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="29" t="s">
         <v>48</v>
       </c>
       <c r="C33" s="4">
@@ -1511,7 +1533,7 @@
       <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="29" t="s">
         <v>48</v>
       </c>
       <c r="C34" s="4">
@@ -1528,17 +1550,17 @@
     <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="37" t="s">
+    <row r="45" spans="1:8" s="45" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
     </row>
     <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
@@ -1547,7 +1569,7 @@
       <c r="A47" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="31" t="s">
         <v>62</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -1561,7 +1583,7 @@
       <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="34" t="s">
+      <c r="B48" s="31" t="s">
         <v>62</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -1575,7 +1597,7 @@
       <c r="A49" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B49" s="34" t="s">
+      <c r="B49" s="31" t="s">
         <v>4</v>
       </c>
       <c r="C49" s="4" t="b">
@@ -1594,23 +1616,23 @@
       <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:8" s="8" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="37" t="s">
+    <row r="53" spans="1:8" s="45" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="42" t="s">
         <v>190</v>
       </c>
-      <c r="B53" s="38"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
     </row>
     <row r="54" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B54" s="34" t="s">
+      <c r="B54" s="31" t="s">
         <v>62</v>
       </c>
       <c r="C54" s="4" t="s">
@@ -1624,7 +1646,7 @@
       <c r="A55" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="31" t="s">
         <v>62</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -1638,7 +1660,7 @@
       <c r="A56" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B56" s="34" t="s">
+      <c r="B56" s="31" t="s">
         <v>4</v>
       </c>
       <c r="C56" s="4" t="b">
@@ -1646,10 +1668,10 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="36" t="s">
+      <c r="A57" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="E57" s="32" t="s">
+      <c r="E57" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F57" s="5">
@@ -1657,10 +1679,10 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="36" t="s">
+      <c r="A58" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="E58" s="32" t="s">
+      <c r="E58" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F58" s="5">
@@ -1672,23 +1694,23 @@
       <c r="A60" s="9"/>
       <c r="C60" s="15"/>
     </row>
-    <row r="61" spans="1:8" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="37" t="s">
+    <row r="61" spans="1:8" s="45" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="B61" s="38"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="38"/>
-      <c r="F61" s="38"/>
-      <c r="G61" s="38"/>
-      <c r="H61" s="38"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="43"/>
     </row>
     <row r="62" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B62" s="33" t="s">
+      <c r="B62" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C62" s="20" t="s">
@@ -1703,7 +1725,7 @@
       <c r="A63" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C63" s="24" t="s">
@@ -1720,7 +1742,7 @@
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B64" s="33" t="s">
+      <c r="B64" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C64" s="20" t="s">
@@ -1737,7 +1759,7 @@
       <c r="A65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B65" s="33" t="s">
+      <c r="B65" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C65" s="20" t="s">
@@ -1751,11 +1773,11 @@
       <c r="A66" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C66" s="47"/>
+      <c r="C66" s="36"/>
       <c r="D66" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E66" s="32" t="s">
+      <c r="E66" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F66" s="5">
@@ -1769,7 +1791,7 @@
       <c r="A67" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B67" s="33" t="s">
+      <c r="B67" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C67" s="20" t="s">
@@ -1786,7 +1808,7 @@
       <c r="A68" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B68" s="33" t="s">
+      <c r="B68" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C68" s="20" t="s">
@@ -1803,7 +1825,7 @@
       <c r="A69" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B69" s="33" t="s">
+      <c r="B69" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C69" s="20" t="s">
@@ -1820,12 +1842,12 @@
       <c r="A70" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B70" s="33" t="s">
+      <c r="B70" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C70" s="20"/>
       <c r="D70" s="19"/>
-      <c r="E70" s="32" t="s">
+      <c r="E70" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F70" s="5">
@@ -1836,14 +1858,14 @@
       <c r="A71" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B71" s="33" t="s">
+      <c r="B71" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C71" s="20"/>
       <c r="D71" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E71" s="32" t="s">
+      <c r="E71" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F71" s="5">
@@ -1854,14 +1876,14 @@
       <c r="A72" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B72" s="33" t="s">
+      <c r="B72" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C72" s="20"/>
       <c r="D72" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E72" s="32" t="s">
+      <c r="E72" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F72" s="5">
@@ -1875,14 +1897,14 @@
       <c r="A73" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B73" s="33" t="s">
+      <c r="B73" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C73" s="20"/>
       <c r="D73" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E73" s="32" t="s">
+      <c r="E73" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F73" s="5">
@@ -1893,14 +1915,14 @@
       <c r="A74" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B74" s="33" t="s">
+      <c r="B74" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C74" s="20"/>
       <c r="D74" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E74" s="32" t="s">
+      <c r="E74" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F74" s="5">
@@ -1911,14 +1933,14 @@
       <c r="A75" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B75" s="33" t="s">
+      <c r="B75" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C75" s="20"/>
       <c r="D75" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E75" s="32" t="s">
+      <c r="E75" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F75" s="5">
@@ -1929,7 +1951,7 @@
       <c r="A76" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B76" s="33" t="s">
+      <c r="B76" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C76" s="20" t="s">
@@ -1943,14 +1965,14 @@
       <c r="A77" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B77" s="33" t="s">
+      <c r="B77" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C77" s="20"/>
       <c r="D77" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E77" s="32" t="s">
+      <c r="E77" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F77" s="5">
@@ -1961,14 +1983,14 @@
       <c r="A78" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B78" s="33" t="s">
+      <c r="B78" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C78" s="20"/>
       <c r="D78" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E78" s="32" t="s">
+      <c r="E78" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F78" s="5">
@@ -1979,7 +2001,7 @@
       <c r="A79" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B79" s="33" t="s">
+      <c r="B79" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C79" s="20"/>
@@ -1991,14 +2013,14 @@
       <c r="A80" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B80" s="33" t="s">
+      <c r="B80" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C80" s="20"/>
       <c r="D80" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E80" s="32" t="s">
+      <c r="E80" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F80" s="5">
@@ -2009,11 +2031,11 @@
       <c r="A81" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C81" s="47"/>
+      <c r="C81" s="36"/>
       <c r="D81" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E81" s="32" t="s">
+      <c r="E81" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F81" s="5">
@@ -2028,7 +2050,7 @@
         <v>161</v>
       </c>
       <c r="C82" s="1"/>
-      <c r="E82" s="32" t="s">
+      <c r="E82" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F82" s="25">
@@ -2043,7 +2065,7 @@
         <v>159</v>
       </c>
       <c r="C83" s="1"/>
-      <c r="E83" s="32" t="s">
+      <c r="E83" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F83" s="5">
@@ -2058,7 +2080,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="1"/>
-      <c r="E84" s="32" t="s">
+      <c r="E84" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F84" s="5">
@@ -2072,21 +2094,21 @@
       <c r="A85" s="9"/>
       <c r="C85" s="15"/>
     </row>
-    <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="40" t="s">
+    <row r="86" spans="1:8" s="48" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="B86" s="41"/>
-      <c r="C86" s="35" t="s">
+      <c r="B86" s="47"/>
+      <c r="C86" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="D86" s="41"/>
-      <c r="E86" s="41"/>
-      <c r="F86" s="34" t="s">
+      <c r="D86" s="51"/>
+      <c r="E86" s="51"/>
+      <c r="F86" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="G86" s="41"/>
-      <c r="H86" s="41"/>
+      <c r="G86" s="47"/>
+      <c r="H86" s="47"/>
     </row>
     <row r="87" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
@@ -2106,7 +2128,7 @@
       </c>
     </row>
     <row r="88" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="27" t="s">
+      <c r="A88" s="38" t="s">
         <v>53</v>
       </c>
       <c r="B88" s="6" t="s">
@@ -2123,7 +2145,7 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="27"/>
+      <c r="A89" s="38"/>
       <c r="B89" s="6" t="s">
         <v>22</v>
       </c>
@@ -2138,7 +2160,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="27"/>
+      <c r="A90" s="38"/>
       <c r="B90" s="6" t="s">
         <v>168</v>
       </c>
@@ -2153,7 +2175,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="27"/>
+      <c r="A91" s="38"/>
       <c r="B91" s="6" t="s">
         <v>138</v>
       </c>
@@ -2168,7 +2190,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="27"/>
+      <c r="A92" s="38"/>
       <c r="B92" s="6" t="s">
         <v>5</v>
       </c>
@@ -2183,7 +2205,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="27"/>
+      <c r="A93" s="38"/>
       <c r="B93" s="6" t="s">
         <v>171</v>
       </c>
@@ -2198,7 +2220,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="27"/>
+      <c r="A94" s="38"/>
       <c r="B94" s="6" t="s">
         <v>31</v>
       </c>
@@ -2213,7 +2235,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="27"/>
+      <c r="A95" s="38"/>
       <c r="B95" s="6" t="s">
         <v>16</v>
       </c>
@@ -2228,7 +2250,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="27"/>
+      <c r="A96" s="38"/>
       <c r="B96" s="6" t="s">
         <v>6</v>
       </c>
@@ -2243,7 +2265,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="27"/>
+      <c r="A97" s="38"/>
       <c r="B97" s="6" t="s">
         <v>8</v>
       </c>
@@ -2258,7 +2280,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="27"/>
+      <c r="A98" s="38"/>
       <c r="B98" s="6" t="s">
         <v>7</v>
       </c>
@@ -2273,7 +2295,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="27"/>
+      <c r="A99" s="38"/>
       <c r="B99" s="6" t="s">
         <v>9</v>
       </c>
@@ -2288,7 +2310,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="27"/>
+      <c r="A100" s="38"/>
       <c r="B100" s="6" t="s">
         <v>11</v>
       </c>
@@ -2303,7 +2325,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="27"/>
+      <c r="A101" s="38"/>
       <c r="B101" s="6" t="s">
         <v>12</v>
       </c>
@@ -2318,7 +2340,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="27"/>
+      <c r="A102" s="38"/>
       <c r="B102" s="6" t="s">
         <v>28</v>
       </c>
@@ -2375,7 +2397,7 @@
       </c>
     </row>
     <row r="106" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="31" t="s">
+      <c r="A106" s="41" t="s">
         <v>189</v>
       </c>
       <c r="B106" s="6" t="s">
@@ -2392,7 +2414,7 @@
       </c>
     </row>
     <row r="107" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="31"/>
+      <c r="A107" s="41"/>
       <c r="B107" s="6" t="s">
         <v>177</v>
       </c>
@@ -2423,28 +2445,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" s="29" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="28"/>
-      <c r="C109" s="30"/>
+    <row r="109" spans="1:8" s="27" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="26"/>
+      <c r="C109" s="28"/>
     </row>
     <row r="110" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="37" t="s">
+    <row r="111" spans="1:8" s="45" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="B111" s="38"/>
-      <c r="C111" s="39"/>
-      <c r="D111" s="38"/>
-      <c r="E111" s="38"/>
-      <c r="F111" s="38"/>
-      <c r="G111" s="38"/>
-      <c r="H111" s="38"/>
+      <c r="B111" s="43"/>
+      <c r="C111" s="44"/>
+      <c r="D111" s="43"/>
+      <c r="E111" s="43"/>
+      <c r="F111" s="43"/>
+      <c r="G111" s="43"/>
+      <c r="H111" s="43"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="32" t="s">
+      <c r="B112" s="29" t="s">
         <v>79</v>
       </c>
       <c r="C112" s="5">
@@ -2455,7 +2477,7 @@
       <c r="A113" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B113" s="32" t="s">
+      <c r="B113" s="29" t="s">
         <v>79</v>
       </c>
       <c r="C113" s="5">
@@ -2469,7 +2491,7 @@
       <c r="A114" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B114" s="32" t="s">
+      <c r="B114" s="29" t="s">
         <v>79</v>
       </c>
       <c r="C114" s="5">
@@ -2483,7 +2505,7 @@
       <c r="A115" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B115" s="32" t="s">
+      <c r="B115" s="29" t="s">
         <v>79</v>
       </c>
       <c r="C115" s="5">
@@ -2507,23 +2529,23 @@
       <c r="C128" s="15"/>
     </row>
     <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A130" s="40" t="s">
+    <row r="130" spans="1:8" s="48" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="B130" s="41"/>
-      <c r="C130" s="42"/>
-      <c r="D130" s="41"/>
-      <c r="E130" s="41"/>
-      <c r="F130" s="41"/>
-      <c r="G130" s="41"/>
-      <c r="H130" s="41"/>
+      <c r="B130" s="47"/>
+      <c r="C130" s="49"/>
+      <c r="D130" s="47"/>
+      <c r="E130" s="47"/>
+      <c r="F130" s="47"/>
+      <c r="G130" s="47"/>
+      <c r="H130" s="47"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C131" s="35" t="s">
+      <c r="C131" s="32" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2658,7 +2680,7 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="A106:A107"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="23">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C18:D18" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C31" xr:uid="{00000000-0002-0000-0000-000001000000}">

</xml_diff>

<commit_message>
New MTS .yml file and update to the .xlsx file
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
+++ b/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa-SET-MTS\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5227D2FB-F1F6-4379-905F-DF761FABC670}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B883C2-0F35-4E86-9D07-C4F5043B6FBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -869,6 +869,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -883,39 +916,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1280,8 +1280,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1298,16 +1298,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -1322,15 +1322,15 @@
     <row r="3" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8" s="35" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34"/>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
@@ -1343,18 +1343,18 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
     </row>
     <row r="7" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
@@ -1377,17 +1377,17 @@
     <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:8" s="45" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="42" t="s">
+    <row r="17" spans="1:8" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -1475,17 +1475,17 @@
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:8" s="45" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="42" t="s">
+    <row r="30" spans="1:8" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="B30" s="43"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
@@ -1550,17 +1550,17 @@
     <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" s="45" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="42" t="s">
+    <row r="45" spans="1:8" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="B45" s="43"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
     </row>
     <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
@@ -1616,17 +1616,17 @@
       <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:8" s="45" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="42" t="s">
+    <row r="53" spans="1:8" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="B53" s="43"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="43"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
     </row>
     <row r="54" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
@@ -1694,17 +1694,17 @@
       <c r="A60" s="9"/>
       <c r="C60" s="15"/>
     </row>
-    <row r="61" spans="1:8" s="45" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="42" t="s">
+    <row r="61" spans="1:8" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="B61" s="43"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="43"/>
-      <c r="E61" s="43"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="43"/>
-      <c r="H61" s="43"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="38"/>
     </row>
     <row r="62" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
@@ -2094,21 +2094,21 @@
       <c r="A85" s="9"/>
       <c r="C85" s="15"/>
     </row>
-    <row r="86" spans="1:8" s="48" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="46" t="s">
+    <row r="86" spans="1:8" s="43" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="B86" s="47"/>
-      <c r="C86" s="50" t="s">
+      <c r="B86" s="42"/>
+      <c r="C86" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D86" s="51"/>
-      <c r="E86" s="51"/>
-      <c r="F86" s="52" t="s">
+      <c r="D86" s="46"/>
+      <c r="E86" s="46"/>
+      <c r="F86" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G86" s="47"/>
-      <c r="H86" s="47"/>
+      <c r="G86" s="42"/>
+      <c r="H86" s="42"/>
     </row>
     <row r="87" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
@@ -2128,7 +2128,7 @@
       </c>
     </row>
     <row r="88" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="38" t="s">
+      <c r="A88" s="49" t="s">
         <v>53</v>
       </c>
       <c r="B88" s="6" t="s">
@@ -2145,7 +2145,7 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="38"/>
+      <c r="A89" s="49"/>
       <c r="B89" s="6" t="s">
         <v>22</v>
       </c>
@@ -2160,7 +2160,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="38"/>
+      <c r="A90" s="49"/>
       <c r="B90" s="6" t="s">
         <v>168</v>
       </c>
@@ -2175,7 +2175,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="38"/>
+      <c r="A91" s="49"/>
       <c r="B91" s="6" t="s">
         <v>138</v>
       </c>
@@ -2190,7 +2190,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="38"/>
+      <c r="A92" s="49"/>
       <c r="B92" s="6" t="s">
         <v>5</v>
       </c>
@@ -2205,7 +2205,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="38"/>
+      <c r="A93" s="49"/>
       <c r="B93" s="6" t="s">
         <v>171</v>
       </c>
@@ -2220,7 +2220,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="38"/>
+      <c r="A94" s="49"/>
       <c r="B94" s="6" t="s">
         <v>31</v>
       </c>
@@ -2235,7 +2235,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="38"/>
+      <c r="A95" s="49"/>
       <c r="B95" s="6" t="s">
         <v>16</v>
       </c>
@@ -2250,7 +2250,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="38"/>
+      <c r="A96" s="49"/>
       <c r="B96" s="6" t="s">
         <v>6</v>
       </c>
@@ -2265,7 +2265,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="38"/>
+      <c r="A97" s="49"/>
       <c r="B97" s="6" t="s">
         <v>8</v>
       </c>
@@ -2280,7 +2280,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="38"/>
+      <c r="A98" s="49"/>
       <c r="B98" s="6" t="s">
         <v>7</v>
       </c>
@@ -2295,7 +2295,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="38"/>
+      <c r="A99" s="49"/>
       <c r="B99" s="6" t="s">
         <v>9</v>
       </c>
@@ -2310,7 +2310,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="38"/>
+      <c r="A100" s="49"/>
       <c r="B100" s="6" t="s">
         <v>11</v>
       </c>
@@ -2325,7 +2325,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="38"/>
+      <c r="A101" s="49"/>
       <c r="B101" s="6" t="s">
         <v>12</v>
       </c>
@@ -2340,7 +2340,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="38"/>
+      <c r="A102" s="49"/>
       <c r="B102" s="6" t="s">
         <v>28</v>
       </c>
@@ -2397,7 +2397,7 @@
       </c>
     </row>
     <row r="106" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="41" t="s">
+      <c r="A106" s="52" t="s">
         <v>189</v>
       </c>
       <c r="B106" s="6" t="s">
@@ -2414,7 +2414,7 @@
       </c>
     </row>
     <row r="107" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="41"/>
+      <c r="A107" s="52"/>
       <c r="B107" s="6" t="s">
         <v>177</v>
       </c>
@@ -2450,17 +2450,17 @@
       <c r="C109" s="28"/>
     </row>
     <row r="110" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" spans="1:8" s="45" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="42" t="s">
+    <row r="111" spans="1:8" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B111" s="43"/>
-      <c r="C111" s="44"/>
-      <c r="D111" s="43"/>
-      <c r="E111" s="43"/>
-      <c r="F111" s="43"/>
-      <c r="G111" s="43"/>
-      <c r="H111" s="43"/>
+      <c r="B111" s="38"/>
+      <c r="C111" s="39"/>
+      <c r="D111" s="38"/>
+      <c r="E111" s="38"/>
+      <c r="F111" s="38"/>
+      <c r="G111" s="38"/>
+      <c r="H111" s="38"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
@@ -2529,17 +2529,17 @@
       <c r="C128" s="15"/>
     </row>
     <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="130" spans="1:8" s="48" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="46" t="s">
+    <row r="130" spans="1:8" s="43" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="41" t="s">
         <v>188</v>
       </c>
-      <c r="B130" s="47"/>
-      <c r="C130" s="49"/>
-      <c r="D130" s="47"/>
-      <c r="E130" s="47"/>
-      <c r="F130" s="47"/>
-      <c r="G130" s="47"/>
-      <c r="H130" s="47"/>
+      <c r="B130" s="42"/>
+      <c r="C130" s="44"/>
+      <c r="D130" s="42"/>
+      <c r="E130" s="42"/>
+      <c r="F130" s="42"/>
+      <c r="G130" s="42"/>
+      <c r="H130" s="42"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">

</xml_diff>

<commit_message>
Duplicate functions now removed from the Build_full_simulation, MTS Zones called directly from the config file
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
+++ b/ConfigFiles/Config_Mid_Term_Scheduling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa-SET-MTS\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B883C2-0F35-4E86-9D07-C4F5043B6FBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5404E13-5367-4DA6-95D3-85B5C23A9551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,22 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$48:$C$54</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="201">
   <si>
     <t>Default value</t>
   </si>
@@ -616,13 +626,28 @@
   </si>
   <si>
     <t>The least amount that customers are willing to recieve to reduce the electricity demand. EUR/MWh</t>
+  </si>
+  <si>
+    <t>MTS</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>True/False Statements</t>
+  </si>
+  <si>
+    <t>Number or Date</t>
+  </si>
+  <si>
+    <t>Active zone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -670,6 +695,15 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -761,7 +795,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -802,9 +836,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -896,12 +927,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -916,12 +941,79 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1280,36 +1372,36 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-    </row>
-    <row r="2" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+    </row>
+    <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1319,44 +1411,44 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:8" s="35" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
-      <c r="B4" s="51" t="s">
+    <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33"/>
+      <c r="B4" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-    </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+    </row>
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="41" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-    </row>
-    <row r="7" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+    </row>
+    <row r="7" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1365,35 +1457,58 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:8" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37" t="s">
+    <row r="8" spans="1:8" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="37"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+    </row>
+    <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="29"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B10" s="30"/>
+    </row>
+    <row r="11" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B11" s="28"/>
+    </row>
+    <row r="12" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:8" s="39" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="29" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1404,11 +1519,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="4" t="b">
@@ -1418,11 +1533,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="4" t="b">
@@ -1432,11 +1547,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="4" t="b">
@@ -1446,80 +1561,80 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>89</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="29" t="s">
         <v>89</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="18" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:8" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="37" t="s">
+    <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:8" s="39" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="17">
         <v>42370</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="17">
         <v>42400</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="28" t="s">
         <v>48</v>
       </c>
       <c r="C33" s="4">
@@ -1529,47 +1644,47 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="28" t="s">
         <v>48</v>
       </c>
       <c r="C34" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="37" t="s">
+    <row r="35" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" s="39" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-    </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="37"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+    </row>
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="30" t="s">
         <v>62</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -1579,11 +1694,11 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="30" t="s">
         <v>62</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -1593,11 +1708,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C49" s="4" t="b">
@@ -1607,32 +1722,32 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:8" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="37" t="s">
+    <row r="52" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:8" s="39" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="B53" s="38"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-    </row>
-    <row r="54" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="37"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+    </row>
+    <row r="54" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B54" s="31" t="s">
+      <c r="B54" s="30" t="s">
         <v>62</v>
       </c>
       <c r="C54" s="4" t="s">
@@ -1642,11 +1757,11 @@
         <v>155</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B55" s="31" t="s">
+      <c r="B55" s="30" t="s">
         <v>62</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -1656,128 +1771,128 @@
         <v>182</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B56" s="31" t="s">
+      <c r="B56" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C56" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="33" t="s">
+    <row r="57" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="E57" s="29" t="s">
+      <c r="E57" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F57" s="5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="33" t="s">
+    <row r="58" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="E58" s="29" t="s">
+      <c r="E58" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F58" s="5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:8" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
-      <c r="C60" s="15"/>
-    </row>
-    <row r="61" spans="1:8" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="37" t="s">
+      <c r="C60" s="14"/>
+    </row>
+    <row r="61" spans="1:8" s="39" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="B61" s="38"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="38"/>
-      <c r="F61" s="38"/>
-      <c r="G61" s="38"/>
-      <c r="H61" s="38"/>
-    </row>
-    <row r="62" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="37"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+    </row>
+    <row r="62" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B62" s="30" t="s">
+      <c r="B62" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C62" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="D62" s="19" t="s">
+      <c r="D62" s="18" t="s">
         <v>92</v>
       </c>
       <c r="H62" s="11"/>
     </row>
-    <row r="63" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="30" t="s">
+      <c r="B63" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C63" s="24" t="s">
+      <c r="C63" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="D63" s="19" t="s">
+      <c r="D63" s="18" t="s">
         <v>92</v>
       </c>
       <c r="H63" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B64" s="30" t="s">
+      <c r="B64" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="18" t="s">
         <v>92</v>
       </c>
       <c r="H64" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B65" s="30" t="s">
+      <c r="B65" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D65" s="19" t="s">
+      <c r="D65" s="18" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C66" s="36"/>
-      <c r="D66" s="19" t="s">
+      <c r="C66" s="35"/>
+      <c r="D66" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E66" s="29" t="s">
+      <c r="E66" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F66" s="5">
@@ -1787,103 +1902,103 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B67" s="30" t="s">
+      <c r="B67" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D67" s="19" t="s">
+      <c r="D67" s="18" t="s">
         <v>92</v>
       </c>
       <c r="H67" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B68" s="30" t="s">
+      <c r="B68" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="D68" s="19" t="s">
+      <c r="D68" s="18" t="s">
         <v>92</v>
       </c>
       <c r="H68" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B69" s="30" t="s">
+      <c r="B69" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="D69" s="19" t="s">
+      <c r="D69" s="18" t="s">
         <v>92</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B70" s="30" t="s">
+      <c r="B70" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C70" s="20"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="29" t="s">
+      <c r="C70" s="19"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F70" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B71" s="30" t="s">
+      <c r="B71" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C71" s="20"/>
-      <c r="D71" s="19" t="s">
+      <c r="C71" s="19"/>
+      <c r="D71" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E71" s="29" t="s">
+      <c r="E71" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F71" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B72" s="30" t="s">
+      <c r="B72" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C72" s="20"/>
-      <c r="D72" s="19" t="s">
+      <c r="C72" s="19"/>
+      <c r="D72" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E72" s="29" t="s">
+      <c r="E72" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F72" s="5">
@@ -1893,149 +2008,149 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B73" s="30" t="s">
+      <c r="B73" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C73" s="20"/>
-      <c r="D73" s="19" t="s">
+      <c r="C73" s="19"/>
+      <c r="D73" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E73" s="29" t="s">
+      <c r="E73" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F73" s="5">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B74" s="30" t="s">
+      <c r="B74" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C74" s="20"/>
-      <c r="D74" s="19" t="s">
+      <c r="C74" s="19"/>
+      <c r="D74" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E74" s="29" t="s">
+      <c r="E74" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F74" s="5">
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B75" s="30" t="s">
+      <c r="B75" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C75" s="20"/>
-      <c r="D75" s="19" t="s">
+      <c r="C75" s="19"/>
+      <c r="D75" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E75" s="29" t="s">
+      <c r="E75" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F75" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B76" s="30" t="s">
+      <c r="B76" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="20" t="s">
+      <c r="C76" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="D76" s="18" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B77" s="30" t="s">
+      <c r="B77" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C77" s="20"/>
-      <c r="D77" s="19" t="s">
+      <c r="C77" s="19"/>
+      <c r="D77" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E77" s="29" t="s">
+      <c r="E77" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F77" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B78" s="30" t="s">
+      <c r="B78" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C78" s="20"/>
-      <c r="D78" s="19" t="s">
+      <c r="C78" s="19"/>
+      <c r="D78" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E78" s="29" t="s">
+      <c r="E78" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F78" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B79" s="30" t="s">
+      <c r="B79" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C79" s="20"/>
-      <c r="D79" s="19" t="s">
+      <c r="C79" s="19"/>
+      <c r="D79" s="18" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B80" s="30" t="s">
+      <c r="B80" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C80" s="20"/>
-      <c r="D80" s="19" t="s">
+      <c r="C80" s="19"/>
+      <c r="D80" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E80" s="29" t="s">
+      <c r="E80" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F80" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C81" s="36"/>
-      <c r="D81" s="19" t="s">
+      <c r="C81" s="35"/>
+      <c r="D81" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E81" s="29" t="s">
+      <c r="E81" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F81" s="5">
@@ -2045,27 +2160,27 @@
         <v>195</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C82" s="1"/>
-      <c r="E82" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="F82" s="25">
+      <c r="E82" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F82" s="24">
         <v>100000</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>159</v>
       </c>
       <c r="C83" s="1"/>
-      <c r="E83" s="29" t="s">
+      <c r="E83" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F83" s="5">
@@ -2075,12 +2190,12 @@
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>162</v>
       </c>
       <c r="C84" s="1"/>
-      <c r="E84" s="29" t="s">
+      <c r="E84" s="28" t="s">
         <v>0</v>
       </c>
       <c r="F84" s="5">
@@ -2090,27 +2205,35 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="9"/>
-      <c r="C85" s="15"/>
-    </row>
-    <row r="86" spans="1:8" s="43" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="41" t="s">
+      <c r="C85" s="14"/>
+    </row>
+    <row r="86" spans="1:8" s="42" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="B86" s="42"/>
-      <c r="C86" s="45" t="s">
+      <c r="B86" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D86" s="46"/>
-      <c r="E86" s="46"/>
-      <c r="F86" s="47" t="s">
+      <c r="C86" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="D86" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="E86" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="G86" s="42"/>
-      <c r="H86" s="42"/>
-    </row>
-    <row r="87" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F86" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="G86" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="H86" s="41"/>
+    </row>
+    <row r="87" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>52</v>
       </c>
@@ -2120,15 +2243,21 @@
       <c r="C87" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D87" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E87" s="6" t="s">
         <v>166</v>
       </c>
       <c r="F87" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="49" t="s">
+      <c r="G87" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="46" t="s">
         <v>53</v>
       </c>
       <c r="B88" s="6" t="s">
@@ -2137,267 +2266,375 @@
       <c r="C88" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D88" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E88" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F88" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="49"/>
+      <c r="G88" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="46"/>
       <c r="B89" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C89" s="4" t="b">
         <v>1</v>
       </c>
+      <c r="D89" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E89" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F89" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="49"/>
+      <c r="G89" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="46"/>
       <c r="B90" s="6" t="s">
         <v>168</v>
       </c>
       <c r="C90" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D90" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E90" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F90" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="49"/>
+      <c r="G90" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="46"/>
       <c r="B91" s="6" t="s">
         <v>138</v>
       </c>
       <c r="C91" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D91" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E91" s="6" t="s">
         <v>169</v>
       </c>
       <c r="F91" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="49"/>
+      <c r="G91" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="46"/>
       <c r="B92" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C92" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D92" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E92" s="6" t="s">
         <v>170</v>
       </c>
       <c r="F92" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="49"/>
+      <c r="G92" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="46"/>
       <c r="B93" s="6" t="s">
         <v>171</v>
       </c>
       <c r="C93" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D93" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E93" s="6" t="s">
         <v>172</v>
       </c>
       <c r="F93" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="49"/>
+      <c r="G93" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="46"/>
       <c r="B94" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C94" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D94" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E94" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F94" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="49"/>
+      <c r="G94" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="46"/>
       <c r="B95" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C95" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D95" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E95" s="6" t="s">
         <v>139</v>
       </c>
       <c r="F95" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="49"/>
+      <c r="G95" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="46"/>
       <c r="B96" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C96" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D96" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E96" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F96" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="49"/>
+      <c r="G96" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="46"/>
       <c r="B97" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C97" s="4" t="b">
         <v>1</v>
       </c>
+      <c r="D97" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E97" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F97" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="49"/>
+      <c r="G97" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="46"/>
       <c r="B98" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C98" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D98" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E98" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F98" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="49"/>
+      <c r="G98" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="46"/>
       <c r="B99" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C99" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D99" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E99" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F99" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="49"/>
+      <c r="G99" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="46"/>
       <c r="B100" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C100" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D100" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E100" s="6" t="s">
         <v>173</v>
       </c>
       <c r="F100" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="49"/>
+      <c r="G100" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="46"/>
       <c r="B101" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C101" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D101" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E101" s="6" t="s">
         <v>174</v>
       </c>
       <c r="F101" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="49"/>
+      <c r="G101" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="46"/>
       <c r="B102" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C102" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D102" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E102" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F102" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G102" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C103" s="4" t="b">
         <v>1</v>
       </c>
+      <c r="D103" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E103" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F103" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G103" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C104" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D104" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E104" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F104" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G104" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C105" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D105" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E105" s="6" t="s">
         <v>175</v>
       </c>
       <c r="F105" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="52" t="s">
+      <c r="G105" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="49" t="s">
         <v>189</v>
       </c>
       <c r="B106" s="6" t="s">
@@ -2406,78 +2643,96 @@
       <c r="C106" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D106" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E106" s="6" t="s">
         <v>176</v>
       </c>
       <c r="F106" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="52"/>
+      <c r="G106" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="49"/>
       <c r="B107" s="6" t="s">
         <v>177</v>
       </c>
       <c r="C107" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D107" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E107" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F107" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="G107" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="H107" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C108" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D108" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E108" s="6" t="s">
         <v>178</v>
       </c>
       <c r="F108" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" s="27" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="26"/>
-      <c r="C109" s="28"/>
-    </row>
-    <row r="110" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" spans="1:8" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="37" t="s">
+      <c r="G108" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" s="26" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="25"/>
+      <c r="C109" s="27"/>
+    </row>
+    <row r="110" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:8" s="39" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="B111" s="38"/>
-      <c r="C111" s="39"/>
-      <c r="D111" s="38"/>
-      <c r="E111" s="38"/>
-      <c r="F111" s="38"/>
-      <c r="G111" s="38"/>
-      <c r="H111" s="38"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B111" s="37"/>
+      <c r="C111" s="38"/>
+      <c r="D111" s="37"/>
+      <c r="E111" s="37"/>
+      <c r="F111" s="37"/>
+      <c r="G111" s="37"/>
+      <c r="H111" s="37"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="29" t="s">
+      <c r="B112" s="28" t="s">
         <v>79</v>
       </c>
       <c r="C112" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B113" s="29" t="s">
+      <c r="B113" s="28" t="s">
         <v>79</v>
       </c>
       <c r="C113" s="5">
@@ -2487,11 +2742,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B114" s="29" t="s">
+      <c r="B114" s="28" t="s">
         <v>79</v>
       </c>
       <c r="C114" s="5">
@@ -2501,175 +2756,175 @@
         <v>82</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B115" s="29" t="s">
+      <c r="B115" s="28" t="s">
         <v>79</v>
       </c>
       <c r="C115" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="128" spans="1:8" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="9"/>
-      <c r="C128" s="15"/>
-    </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="130" spans="1:8" s="43" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="41" t="s">
+      <c r="C128" s="14"/>
+    </row>
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="1:8" s="42" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="B130" s="42"/>
-      <c r="C130" s="44"/>
-      <c r="D130" s="42"/>
-      <c r="E130" s="42"/>
-      <c r="F130" s="42"/>
-      <c r="G130" s="42"/>
-      <c r="H130" s="42"/>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B130" s="41"/>
+      <c r="C130" s="43"/>
+      <c r="D130" s="41"/>
+      <c r="E130" s="41"/>
+      <c r="F130" s="41"/>
+      <c r="G130" s="41"/>
+      <c r="H130" s="41"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C131" s="32" t="s">
+      <c r="C131" s="31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B132" s="23" t="s">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="C132" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B133" s="23" t="s">
+      <c r="C132" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C133" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B134" s="23" t="s">
+      <c r="C133" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B134" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="C134" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B135" s="23" t="s">
+      <c r="C134" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C135" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B136" s="23" t="s">
+      <c r="C135" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C136" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B137" s="23" t="s">
+      <c r="C136" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B137" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="C137" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B138" s="23" t="s">
+      <c r="C137" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B138" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C138" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B139" s="23" t="s">
+      <c r="C138" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B139" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="C139" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B140" s="23" t="s">
+      <c r="C139" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B140" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="C140" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B141" s="23" t="s">
+      <c r="C140" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B141" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="C141" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B142" s="23" t="s">
+      <c r="C141" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B142" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="C142" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B143" s="23" t="s">
+      <c r="C142" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B143" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="C143" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B144" s="23" t="s">
+      <c r="C143" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B144" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="C144" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B145" s="23" t="s">
+      <c r="C144" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B145" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="C145" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B146" s="23" t="s">
+      <c r="C145" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B146" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="C146" s="22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="C146" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F165" s="2"/>
     </row>
   </sheetData>
@@ -2681,6 +2936,22 @@
     <mergeCell ref="A106:A107"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="C87:D108 F87:G108 C49 C19:C21 C132:C146">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="23">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C18:D18" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C31" xr:uid="{00000000-0002-0000-0000-000001000000}">
@@ -2722,12 +2993,12 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000011000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C132:C146 C87:C108 F87:F108</xm:sqref>
+          <xm:sqref>C132:C146 C87:D108 F87:G108</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write excel files" prompt="If set to true, one excel file per parameter will be written in the simulation environment directory." xr:uid="{00000000-0002-0000-0000-000012000000}">
           <x14:formula1>
@@ -2771,12 +3042,6 @@
           </x14:formula1>
           <xm:sqref>C54</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0512806B-C050-4E95-821E-3CF48A786E8B}">
-          <x14:formula1>
-            <xm:f>[ConfigEU.xlsx]Lists!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>G88:G102</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hydro scheduling horizon" prompt="Annual: Performes hydro scheduling for one year_x000a_Stop-date driven: Performes hydro scheduling between Start and Stop dates_x000a_" xr:uid="{345F7B42-F54C-4808-919E-6CF06ADB107C}">
           <x14:formula1>
             <xm:f>Lists!$F$2:$F$5</xm:f>
@@ -2804,36 +3069,36 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>44</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2853,7 +3118,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2870,7 +3135,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -2881,7 +3146,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>137</v>
       </c>
@@ -2889,7 +3154,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>140</v>
       </c>
@@ -2906,760 +3171,760 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="17"/>
+    <col min="1" max="1" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="B2" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="B3" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="B4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="B5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="B6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" s="20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="B7" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="B8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O9" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="B9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="B10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O11" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="B11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="B12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O13" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
+      <c r="B13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N14" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O14" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+      <c r="B14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O15" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="B15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O16" s="21" t="b">
+      <c r="B16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="20" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3667,6 +3932,14 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:D30">
     <sortCondition ref="D1"/>
   </sortState>
+  <conditionalFormatting sqref="B2:O16">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>